<commit_message>
Update Leave Card 2/2/2024 4:33 PM
</commit_message>
<xml_diff>
--- a/CASUAL/LA CENRO/FLORES, RICHARD.xlsx
+++ b/CASUAL/LA CENRO/FLORES, RICHARD.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA CENRO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\dole-pc\Users\DOLE\Desktop\LEAVE-CARD\CASUAL\LA CENRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EF8804-9E47-413F-886C-6628E24B7DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018 LEAVE CREDITS" sheetId="4" r:id="rId1"/>
@@ -26,7 +27,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'2017 LEAVE BALANCE'!$1:$9</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'2018 LEAVE CREDITS'!$1:$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="99">
   <si>
     <t>PERIOD</t>
   </si>
@@ -324,12 +325,21 @@
   </si>
   <si>
     <t>UT(0-2-16)</t>
+  </si>
+  <si>
+    <t>TOTAL LEAVE BALANCE</t>
+  </si>
+  <si>
+    <t>GSO</t>
+  </si>
+  <si>
+    <t>FLORES, RICHARD A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
@@ -708,14 +718,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -725,9 +738,6 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1239,7 +1249,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -1256,25 +1266,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A8:K130" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="A8:K130" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="25"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="24"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="23"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="22"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PERIOD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="PARTICULARS" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="EARNED" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BALANCE" dataDxfId="21">
       <calculatedColumnFormula>SUM(Table13[EARNED])-SUM(Table13[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="20"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="19">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="EARNED " dataDxfId="19">
       <calculatedColumnFormula>IF(ISBLANK(Table13[[#This Row],[EARNED]]),"",Table13[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="BALANCE " dataDxfId="17">
       <calculatedColumnFormula>SUM(Table13[[EARNED ]])-SUM(Table13[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="REMARKS" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1286,25 +1296,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A8:K75" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:K75" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <tableColumns count="11">
-    <tableColumn id="1" name="PERIOD" dataDxfId="10"/>
-    <tableColumn id="2" name="PARTICULARS" dataDxfId="9"/>
-    <tableColumn id="3" name="EARNED" dataDxfId="8"/>
-    <tableColumn id="4" name="Absence Undertime W/ Pay" dataDxfId="7"/>
-    <tableColumn id="5" name="BALANCE" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="PERIOD" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="PARTICULARS" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="EARNED" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Absence Undertime W/ Pay" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="BALANCE" dataDxfId="6">
       <calculatedColumnFormula>SUM(Table1[EARNED])-SUM(Table1[Absence Undertime W/ Pay])+CONVERTION!$A$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Absence Undertime W/O Pay" dataDxfId="5"/>
-    <tableColumn id="7" name="EARNED " dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Absence Undertime W/O Pay" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="EARNED " dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(Table1[[#This Row],[EARNED]]),"",Table1[[#This Row],[EARNED]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
-    <tableColumn id="9" name="BALANCE " dataDxfId="2">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Absence Undertime  W/ Pay" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="BALANCE " dataDxfId="2">
       <calculatedColumnFormula>SUM(Table1[[EARNED ]])-SUM(Table1[Absence Undertime  W/ Pay])+CONVERTION!$B$3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
-    <tableColumn id="11" name="REMARKS" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="Absence Undertime  W/O Pay" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="REMARKS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1611,55 +1621,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A58" activePane="bottomLeft"/>
-      <selection activeCell="O8" sqref="O8"/>
+      <pane ySplit="3696" topLeftCell="A58"/>
+      <selection activeCell="D9" sqref="D9:D130"/>
       <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>42</v>
+        <v>98</v>
       </c>
       <c r="C2" s="50"/>
       <c r="D2" s="21" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -1668,16 +1678,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="52"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -1688,16 +1698,18 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
+      <c r="F4" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -1705,7 +1717,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -1718,24 +1730,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -1770,7 +1782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -1794,7 +1806,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>44</v>
       </c>
@@ -1816,7 +1828,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>43101</v>
       </c>
@@ -1836,7 +1848,7 @@
       <c r="J11" s="11"/>
       <c r="K11" s="20"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="40">
         <v>43132</v>
       </c>
@@ -1856,7 +1868,7 @@
       <c r="J12" s="11"/>
       <c r="K12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <v>43160</v>
       </c>
@@ -1876,7 +1888,7 @@
       <c r="J13" s="11"/>
       <c r="K13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="40">
         <v>43191</v>
       </c>
@@ -1896,7 +1908,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <v>43221</v>
       </c>
@@ -1916,7 +1928,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="41">
         <v>43252</v>
       </c>
@@ -1936,7 +1948,7 @@
       <c r="J16" s="12"/>
       <c r="K16" s="15"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
         <v>43282</v>
       </c>
@@ -1956,7 +1968,7 @@
       <c r="J17" s="11"/>
       <c r="K17" s="20"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <f>EDATE(A17,1)</f>
         <v>43313</v>
@@ -1977,7 +1989,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="40">
         <f>EDATE(A18,1)</f>
         <v>43344</v>
@@ -1998,7 +2010,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
         <v>43374</v>
       </c>
@@ -2018,7 +2030,7 @@
       <c r="J20" s="11"/>
       <c r="K20" s="20"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="40">
         <v>43405</v>
       </c>
@@ -2038,7 +2050,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40">
         <v>43435</v>
       </c>
@@ -2062,7 +2074,7 @@
       <c r="J22" s="11"/>
       <c r="K22" s="49"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="48" t="s">
         <v>48</v>
       </c>
@@ -2080,7 +2092,7 @@
       <c r="J23" s="11"/>
       <c r="K23" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="40">
         <v>43466</v>
       </c>
@@ -2100,7 +2112,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <v>43497</v>
       </c>
@@ -2126,7 +2138,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40">
         <v>43525</v>
       </c>
@@ -2152,7 +2164,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <v>43556</v>
       </c>
@@ -2172,7 +2184,7 @@
       <c r="J27" s="11"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40">
         <v>43586</v>
       </c>
@@ -2192,7 +2204,7 @@
       <c r="J28" s="11"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40">
         <v>43617</v>
       </c>
@@ -2212,7 +2224,7 @@
       <c r="J29" s="11"/>
       <c r="K29" s="20"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40">
         <v>43647</v>
       </c>
@@ -2232,7 +2244,7 @@
       <c r="J30" s="11"/>
       <c r="K30" s="20"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40">
         <v>43678</v>
       </c>
@@ -2252,7 +2264,7 @@
       <c r="J31" s="11"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <v>43709</v>
       </c>
@@ -2272,7 +2284,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
         <v>43739</v>
       </c>
@@ -2292,7 +2304,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="20"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <v>43770</v>
       </c>
@@ -2312,7 +2324,7 @@
       <c r="J34" s="11"/>
       <c r="K34" s="20"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
         <v>43800</v>
       </c>
@@ -2332,7 +2344,7 @@
       <c r="J35" s="11"/>
       <c r="K35" s="20"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="48" t="s">
         <v>58</v>
       </c>
@@ -2350,7 +2362,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40">
         <v>43831</v>
       </c>
@@ -2370,7 +2382,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40">
         <v>43862</v>
       </c>
@@ -2390,7 +2402,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40">
         <v>43891</v>
       </c>
@@ -2410,7 +2422,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40">
         <v>43922</v>
       </c>
@@ -2430,7 +2442,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40">
         <v>43952</v>
       </c>
@@ -2450,7 +2462,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40">
         <v>43983</v>
       </c>
@@ -2470,7 +2482,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40">
         <v>44013</v>
       </c>
@@ -2490,7 +2502,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40">
         <v>44044</v>
       </c>
@@ -2510,7 +2522,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40">
         <v>44075</v>
       </c>
@@ -2530,7 +2542,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40">
         <v>44105</v>
       </c>
@@ -2550,7 +2562,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40">
         <v>44136</v>
       </c>
@@ -2570,7 +2582,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40">
         <v>44166</v>
       </c>
@@ -2594,7 +2606,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="48" t="s">
         <v>60</v>
       </c>
@@ -2612,7 +2624,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40">
         <v>44197</v>
       </c>
@@ -2632,7 +2644,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40">
         <v>44228</v>
       </c>
@@ -2652,7 +2664,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40">
         <v>44256</v>
       </c>
@@ -2672,7 +2684,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40">
         <v>44287</v>
       </c>
@@ -2692,7 +2704,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40">
         <v>44317</v>
       </c>
@@ -2712,7 +2724,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40">
         <v>44348</v>
       </c>
@@ -2732,7 +2744,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40">
         <v>44378</v>
       </c>
@@ -2752,7 +2764,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40">
         <v>44409</v>
       </c>
@@ -2772,7 +2784,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40">
         <v>44440</v>
       </c>
@@ -2792,7 +2804,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40">
         <v>44470</v>
       </c>
@@ -2812,7 +2824,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40">
         <v>44501</v>
       </c>
@@ -2832,7 +2844,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40">
         <v>44531</v>
       </c>
@@ -2856,7 +2868,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="48" t="s">
         <v>61</v>
       </c>
@@ -2874,7 +2886,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40">
         <v>44562</v>
       </c>
@@ -2894,7 +2906,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40">
         <v>44593</v>
       </c>
@@ -2914,7 +2926,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40">
         <v>44621</v>
       </c>
@@ -2940,7 +2952,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40"/>
       <c r="B66" s="20" t="s">
         <v>95</v>
@@ -2960,7 +2972,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40">
         <v>44652</v>
       </c>
@@ -2984,7 +2996,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40">
         <v>44682</v>
       </c>
@@ -3010,7 +3022,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40"/>
       <c r="B69" s="20" t="s">
         <v>90</v>
@@ -3032,7 +3044,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40"/>
       <c r="B70" s="20" t="s">
         <v>92</v>
@@ -3052,7 +3064,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40">
         <v>44713</v>
       </c>
@@ -3078,7 +3090,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40"/>
       <c r="B72" s="20" t="s">
         <v>89</v>
@@ -3098,7 +3110,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40">
         <v>44743</v>
       </c>
@@ -3122,7 +3134,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40">
         <v>44774</v>
       </c>
@@ -3146,7 +3158,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="40">
         <v>44805</v>
       </c>
@@ -3172,7 +3184,7 @@
         <v>44813</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="40"/>
       <c r="B76" s="20" t="s">
         <v>84</v>
@@ -3192,7 +3204,7 @@
       <c r="J76" s="11"/>
       <c r="K76" s="49"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="40">
         <v>44835</v>
       </c>
@@ -3218,7 +3230,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="40"/>
       <c r="B78" s="20" t="s">
         <v>83</v>
@@ -3238,7 +3250,7 @@
       <c r="J78" s="11"/>
       <c r="K78" s="20"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="40">
         <v>44866</v>
       </c>
@@ -3264,7 +3276,7 @@
         <v>44872</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="40"/>
       <c r="B80" s="20" t="s">
         <v>80</v>
@@ -3284,7 +3296,7 @@
       <c r="J80" s="11"/>
       <c r="K80" s="49"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="40">
         <v>44896</v>
       </c>
@@ -3310,7 +3322,7 @@
         <v>44912</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="40"/>
       <c r="B82" s="20" t="s">
         <v>78</v>
@@ -3330,7 +3342,7 @@
       <c r="J82" s="11"/>
       <c r="K82" s="49"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="48" t="s">
         <v>66</v>
       </c>
@@ -3348,7 +3360,7 @@
       <c r="J83" s="11"/>
       <c r="K83" s="20"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="40">
         <v>44957</v>
       </c>
@@ -3368,7 +3380,7 @@
       <c r="J84" s="11"/>
       <c r="K84" s="20"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" s="40">
         <v>44985</v>
       </c>
@@ -3388,7 +3400,7 @@
       <c r="J85" s="11"/>
       <c r="K85" s="20"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" s="40">
         <v>45016</v>
       </c>
@@ -3410,7 +3422,7 @@
       <c r="J86" s="11"/>
       <c r="K86" s="20"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" s="40">
         <v>45046</v>
       </c>
@@ -3430,7 +3442,7 @@
       <c r="J87" s="11"/>
       <c r="K87" s="20"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="40">
         <v>45077</v>
       </c>
@@ -3450,7 +3462,7 @@
       <c r="J88" s="11"/>
       <c r="K88" s="20"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="40">
         <v>45107</v>
       </c>
@@ -3470,7 +3482,7 @@
       <c r="J89" s="11"/>
       <c r="K89" s="20"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="40">
         <v>45108</v>
       </c>
@@ -3490,7 +3502,7 @@
       <c r="J90" s="11"/>
       <c r="K90" s="20"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="40">
         <v>45139</v>
       </c>
@@ -3510,7 +3522,7 @@
       <c r="J91" s="11"/>
       <c r="K91" s="20"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="40">
         <v>45170</v>
       </c>
@@ -3530,7 +3542,7 @@
       <c r="J92" s="11"/>
       <c r="K92" s="20"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="40">
         <v>45200</v>
       </c>
@@ -3550,7 +3562,7 @@
       <c r="J93" s="11"/>
       <c r="K93" s="20"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="40">
         <v>45231</v>
       </c>
@@ -3568,7 +3580,7 @@
       <c r="J94" s="11"/>
       <c r="K94" s="20"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="40">
         <v>45261</v>
       </c>
@@ -3586,7 +3598,7 @@
       <c r="J95" s="11"/>
       <c r="K95" s="20"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="40"/>
       <c r="B96" s="20"/>
       <c r="C96" s="13"/>
@@ -3602,7 +3614,7 @@
       <c r="J96" s="11"/>
       <c r="K96" s="20"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A97" s="40"/>
       <c r="B97" s="20"/>
       <c r="C97" s="13"/>
@@ -3618,7 +3630,7 @@
       <c r="J97" s="11"/>
       <c r="K97" s="20"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A98" s="40"/>
       <c r="B98" s="20"/>
       <c r="C98" s="13"/>
@@ -3634,7 +3646,7 @@
       <c r="J98" s="11"/>
       <c r="K98" s="20"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A99" s="40"/>
       <c r="B99" s="20"/>
       <c r="C99" s="13"/>
@@ -3650,7 +3662,7 @@
       <c r="J99" s="11"/>
       <c r="K99" s="20"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A100" s="40"/>
       <c r="B100" s="20"/>
       <c r="C100" s="13"/>
@@ -3666,7 +3678,7 @@
       <c r="J100" s="11"/>
       <c r="K100" s="20"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A101" s="40"/>
       <c r="B101" s="20"/>
       <c r="C101" s="13"/>
@@ -3682,7 +3694,7 @@
       <c r="J101" s="11"/>
       <c r="K101" s="20"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A102" s="40"/>
       <c r="B102" s="20"/>
       <c r="C102" s="13"/>
@@ -3698,7 +3710,7 @@
       <c r="J102" s="11"/>
       <c r="K102" s="20"/>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A103" s="40"/>
       <c r="B103" s="20"/>
       <c r="C103" s="13"/>
@@ -3714,7 +3726,7 @@
       <c r="J103" s="11"/>
       <c r="K103" s="20"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A104" s="40"/>
       <c r="B104" s="20"/>
       <c r="C104" s="13"/>
@@ -3730,7 +3742,7 @@
       <c r="J104" s="11"/>
       <c r="K104" s="20"/>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A105" s="40"/>
       <c r="B105" s="20"/>
       <c r="C105" s="13"/>
@@ -3746,7 +3758,7 @@
       <c r="J105" s="11"/>
       <c r="K105" s="20"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A106" s="40"/>
       <c r="B106" s="20"/>
       <c r="C106" s="13"/>
@@ -3762,7 +3774,7 @@
       <c r="J106" s="11"/>
       <c r="K106" s="20"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A107" s="40"/>
       <c r="B107" s="20"/>
       <c r="C107" s="13"/>
@@ -3778,7 +3790,7 @@
       <c r="J107" s="11"/>
       <c r="K107" s="20"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A108" s="40"/>
       <c r="B108" s="20"/>
       <c r="C108" s="13"/>
@@ -3794,7 +3806,7 @@
       <c r="J108" s="11"/>
       <c r="K108" s="20"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A109" s="40"/>
       <c r="B109" s="20"/>
       <c r="C109" s="13"/>
@@ -3810,7 +3822,7 @@
       <c r="J109" s="11"/>
       <c r="K109" s="20"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A110" s="40"/>
       <c r="B110" s="20"/>
       <c r="C110" s="13"/>
@@ -3826,7 +3838,7 @@
       <c r="J110" s="11"/>
       <c r="K110" s="20"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A111" s="40"/>
       <c r="B111" s="20"/>
       <c r="C111" s="13"/>
@@ -3842,7 +3854,7 @@
       <c r="J111" s="11"/>
       <c r="K111" s="20"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A112" s="40"/>
       <c r="B112" s="20"/>
       <c r="C112" s="13"/>
@@ -3858,7 +3870,7 @@
       <c r="J112" s="11"/>
       <c r="K112" s="20"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="40"/>
       <c r="B113" s="20"/>
       <c r="C113" s="13"/>
@@ -3874,7 +3886,7 @@
       <c r="J113" s="11"/>
       <c r="K113" s="20"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="40"/>
       <c r="B114" s="20"/>
       <c r="C114" s="13"/>
@@ -3890,7 +3902,7 @@
       <c r="J114" s="11"/>
       <c r="K114" s="20"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="40"/>
       <c r="B115" s="20"/>
       <c r="C115" s="13"/>
@@ -3906,7 +3918,7 @@
       <c r="J115" s="11"/>
       <c r="K115" s="20"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="40"/>
       <c r="B116" s="20"/>
       <c r="C116" s="13"/>
@@ -3922,7 +3934,7 @@
       <c r="J116" s="11"/>
       <c r="K116" s="20"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="40"/>
       <c r="B117" s="20"/>
       <c r="C117" s="13"/>
@@ -3938,7 +3950,7 @@
       <c r="J117" s="11"/>
       <c r="K117" s="20"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="40"/>
       <c r="B118" s="20"/>
       <c r="C118" s="13"/>
@@ -3954,7 +3966,7 @@
       <c r="J118" s="11"/>
       <c r="K118" s="20"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="40"/>
       <c r="B119" s="20"/>
       <c r="C119" s="13"/>
@@ -3970,7 +3982,7 @@
       <c r="J119" s="11"/>
       <c r="K119" s="20"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="40"/>
       <c r="B120" s="20"/>
       <c r="C120" s="13"/>
@@ -3986,7 +3998,7 @@
       <c r="J120" s="11"/>
       <c r="K120" s="20"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A121" s="40"/>
       <c r="B121" s="20"/>
       <c r="C121" s="13"/>
@@ -4002,7 +4014,7 @@
       <c r="J121" s="11"/>
       <c r="K121" s="20"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="40"/>
       <c r="B122" s="20"/>
       <c r="C122" s="13"/>
@@ -4018,7 +4030,7 @@
       <c r="J122" s="11"/>
       <c r="K122" s="20"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="40"/>
       <c r="B123" s="20"/>
       <c r="C123" s="13"/>
@@ -4034,7 +4046,7 @@
       <c r="J123" s="11"/>
       <c r="K123" s="20"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="40"/>
       <c r="B124" s="20"/>
       <c r="C124" s="13"/>
@@ -4050,7 +4062,7 @@
       <c r="J124" s="11"/>
       <c r="K124" s="20"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="40"/>
       <c r="B125" s="20"/>
       <c r="C125" s="13"/>
@@ -4066,7 +4078,7 @@
       <c r="J125" s="11"/>
       <c r="K125" s="20"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="40"/>
       <c r="B126" s="20"/>
       <c r="C126" s="13"/>
@@ -4082,7 +4094,7 @@
       <c r="J126" s="11"/>
       <c r="K126" s="20"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="40"/>
       <c r="B127" s="20"/>
       <c r="C127" s="13"/>
@@ -4098,7 +4110,7 @@
       <c r="J127" s="11"/>
       <c r="K127" s="20"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="40"/>
       <c r="B128" s="20"/>
       <c r="C128" s="13"/>
@@ -4114,7 +4126,7 @@
       <c r="J128" s="11"/>
       <c r="K128" s="20"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A129" s="40"/>
       <c r="B129" s="20"/>
       <c r="C129" s="13"/>
@@ -4130,7 +4142,7 @@
       <c r="J129" s="11"/>
       <c r="K129" s="20"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A130" s="41"/>
       <c r="B130" s="15"/>
       <c r="C130" s="42"/>
@@ -4148,23 +4160,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4187,34 +4199,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:K75"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3690" topLeftCell="A16" activePane="bottomLeft"/>
+      <pane ySplit="3696" topLeftCell="A4" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F4:G4"/>
       <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="30" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
@@ -4226,16 +4238,16 @@
         <v>14</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="25"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J2" s="51"/>
+      <c r="K2" s="52"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>15</v>
       </c>
@@ -4244,16 +4256,16 @@
       <c r="D3" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="52"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="26"/>
-      <c r="J3" s="55"/>
-      <c r="K3" s="56"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
@@ -4264,18 +4276,18 @@
       <c r="D4" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="52" t="s">
+      <c r="F4" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="52"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="26"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="53"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="51"/>
+      <c r="K4" s="52"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="H5" s="27" t="s">
         <v>18</v>
@@ -4283,7 +4295,7 @@
       <c r="I5" s="27"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31"/>
@@ -4296,24 +4308,24 @@
       <c r="J6" s="8"/>
       <c r="K6" s="19"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
       <c r="K7" s="14"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
@@ -4348,7 +4360,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="24" t="s">
         <v>23</v>
@@ -4372,7 +4384,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>44</v>
       </c>
@@ -4394,7 +4406,7 @@
       <c r="J10" s="11"/>
       <c r="K10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="40">
         <v>43221</v>
       </c>
@@ -4418,7 +4430,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="41">
         <v>43252</v>
       </c>
@@ -4442,7 +4454,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="40">
         <v>43435</v>
       </c>
@@ -4466,7 +4478,7 @@
         <v>43440</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="48" t="s">
         <v>48</v>
       </c>
@@ -4484,7 +4496,7 @@
       <c r="J14" s="11"/>
       <c r="K14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="40">
         <v>43678</v>
       </c>
@@ -4506,7 +4518,7 @@
       <c r="J15" s="11"/>
       <c r="K15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="40">
         <v>43709</v>
       </c>
@@ -4530,7 +4542,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="40">
         <v>43770</v>
       </c>
@@ -4554,7 +4566,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="40">
         <v>43800</v>
       </c>
@@ -4572,7 +4584,7 @@
       <c r="J18" s="11"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="48" t="s">
         <v>58</v>
       </c>
@@ -4590,7 +4602,7 @@
       <c r="J19" s="11"/>
       <c r="K19" s="20"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="40">
         <v>43862</v>
       </c>
@@ -4614,7 +4626,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="48" t="s">
         <v>61</v>
       </c>
@@ -4632,7 +4644,7 @@
       <c r="J21" s="11"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="40">
         <v>44743</v>
       </c>
@@ -4656,7 +4668,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="40">
         <v>44774</v>
       </c>
@@ -4680,7 +4692,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="48" t="s">
         <v>66</v>
       </c>
@@ -4698,7 +4710,7 @@
       <c r="J24" s="11"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <v>44927</v>
       </c>
@@ -4722,7 +4734,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="40"/>
       <c r="B26" s="20" t="s">
         <v>55</v>
@@ -4744,7 +4756,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="40">
         <v>45047</v>
       </c>
@@ -4768,7 +4780,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="40"/>
       <c r="B28" s="20" t="s">
         <v>45</v>
@@ -4790,7 +4802,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="40"/>
       <c r="B29" s="20" t="s">
         <v>45</v>
@@ -4812,7 +4824,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="40">
         <v>45078</v>
       </c>
@@ -4836,7 +4848,7 @@
         <v>45090</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="40"/>
       <c r="B31" s="20" t="s">
         <v>53</v>
@@ -4858,7 +4870,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="40">
         <v>45108</v>
       </c>
@@ -4882,7 +4894,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="40">
         <v>45153</v>
       </c>
@@ -4906,7 +4918,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="40">
         <v>45170</v>
       </c>
@@ -4930,7 +4942,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="40">
         <v>45200</v>
       </c>
@@ -4954,7 +4966,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="40"/>
       <c r="B36" s="20"/>
       <c r="C36" s="13"/>
@@ -4970,7 +4982,7 @@
       <c r="J36" s="11"/>
       <c r="K36" s="20"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="40"/>
       <c r="B37" s="20"/>
       <c r="C37" s="13"/>
@@ -4986,7 +4998,7 @@
       <c r="J37" s="11"/>
       <c r="K37" s="20"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="40"/>
       <c r="B38" s="20"/>
       <c r="C38" s="13"/>
@@ -5002,7 +5014,7 @@
       <c r="J38" s="11"/>
       <c r="K38" s="20"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="40"/>
       <c r="B39" s="20"/>
       <c r="C39" s="13"/>
@@ -5018,7 +5030,7 @@
       <c r="J39" s="11"/>
       <c r="K39" s="20"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="40"/>
       <c r="B40" s="20"/>
       <c r="C40" s="13"/>
@@ -5034,7 +5046,7 @@
       <c r="J40" s="11"/>
       <c r="K40" s="20"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="40"/>
       <c r="B41" s="20"/>
       <c r="C41" s="13"/>
@@ -5050,7 +5062,7 @@
       <c r="J41" s="11"/>
       <c r="K41" s="20"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="40"/>
       <c r="B42" s="20"/>
       <c r="C42" s="13"/>
@@ -5066,7 +5078,7 @@
       <c r="J42" s="11"/>
       <c r="K42" s="20"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="40"/>
       <c r="B43" s="20"/>
       <c r="C43" s="13"/>
@@ -5082,7 +5094,7 @@
       <c r="J43" s="11"/>
       <c r="K43" s="20"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="40"/>
       <c r="B44" s="20"/>
       <c r="C44" s="13"/>
@@ -5098,7 +5110,7 @@
       <c r="J44" s="11"/>
       <c r="K44" s="20"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="40"/>
       <c r="B45" s="20"/>
       <c r="C45" s="13"/>
@@ -5114,7 +5126,7 @@
       <c r="J45" s="11"/>
       <c r="K45" s="20"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="40"/>
       <c r="B46" s="20"/>
       <c r="C46" s="13"/>
@@ -5130,7 +5142,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="20"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="40"/>
       <c r="B47" s="20"/>
       <c r="C47" s="13"/>
@@ -5146,7 +5158,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="20"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="40"/>
       <c r="B48" s="20"/>
       <c r="C48" s="13"/>
@@ -5162,7 +5174,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="20"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="40"/>
       <c r="B49" s="20"/>
       <c r="C49" s="13"/>
@@ -5178,7 +5190,7 @@
       <c r="J49" s="11"/>
       <c r="K49" s="20"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="40"/>
       <c r="B50" s="20"/>
       <c r="C50" s="13"/>
@@ -5194,7 +5206,7 @@
       <c r="J50" s="11"/>
       <c r="K50" s="20"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="40"/>
       <c r="B51" s="20"/>
       <c r="C51" s="13"/>
@@ -5210,7 +5222,7 @@
       <c r="J51" s="11"/>
       <c r="K51" s="20"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="40"/>
       <c r="B52" s="20"/>
       <c r="C52" s="13"/>
@@ -5226,7 +5238,7 @@
       <c r="J52" s="11"/>
       <c r="K52" s="20"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="40"/>
       <c r="B53" s="20"/>
       <c r="C53" s="13"/>
@@ -5242,7 +5254,7 @@
       <c r="J53" s="11"/>
       <c r="K53" s="20"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="40"/>
       <c r="B54" s="20"/>
       <c r="C54" s="13"/>
@@ -5258,7 +5270,7 @@
       <c r="J54" s="11"/>
       <c r="K54" s="20"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
       <c r="B55" s="20"/>
       <c r="C55" s="13"/>
@@ -5274,7 +5286,7 @@
       <c r="J55" s="11"/>
       <c r="K55" s="20"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="40"/>
       <c r="B56" s="20"/>
       <c r="C56" s="13"/>
@@ -5290,7 +5302,7 @@
       <c r="J56" s="11"/>
       <c r="K56" s="20"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="40"/>
       <c r="B57" s="20"/>
       <c r="C57" s="13"/>
@@ -5306,7 +5318,7 @@
       <c r="J57" s="11"/>
       <c r="K57" s="20"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="40"/>
       <c r="B58" s="20"/>
       <c r="C58" s="13"/>
@@ -5322,7 +5334,7 @@
       <c r="J58" s="11"/>
       <c r="K58" s="20"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="40"/>
       <c r="B59" s="20"/>
       <c r="C59" s="13"/>
@@ -5338,7 +5350,7 @@
       <c r="J59" s="11"/>
       <c r="K59" s="20"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="40"/>
       <c r="B60" s="20"/>
       <c r="C60" s="13"/>
@@ -5354,7 +5366,7 @@
       <c r="J60" s="11"/>
       <c r="K60" s="20"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="40"/>
       <c r="B61" s="20"/>
       <c r="C61" s="13"/>
@@ -5370,7 +5382,7 @@
       <c r="J61" s="11"/>
       <c r="K61" s="20"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="40"/>
       <c r="B62" s="20"/>
       <c r="C62" s="13"/>
@@ -5386,7 +5398,7 @@
       <c r="J62" s="11"/>
       <c r="K62" s="20"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="40"/>
       <c r="B63" s="20"/>
       <c r="C63" s="13"/>
@@ -5402,7 +5414,7 @@
       <c r="J63" s="11"/>
       <c r="K63" s="20"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="40"/>
       <c r="B64" s="20"/>
       <c r="C64" s="13"/>
@@ -5418,7 +5430,7 @@
       <c r="J64" s="11"/>
       <c r="K64" s="20"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="40"/>
       <c r="B65" s="20"/>
       <c r="C65" s="13"/>
@@ -5434,7 +5446,7 @@
       <c r="J65" s="11"/>
       <c r="K65" s="20"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="40"/>
       <c r="B66" s="20"/>
       <c r="C66" s="13"/>
@@ -5450,7 +5462,7 @@
       <c r="J66" s="11"/>
       <c r="K66" s="20"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="40"/>
       <c r="B67" s="20"/>
       <c r="C67" s="13"/>
@@ -5466,7 +5478,7 @@
       <c r="J67" s="11"/>
       <c r="K67" s="20"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="40"/>
       <c r="B68" s="20"/>
       <c r="C68" s="13"/>
@@ -5482,7 +5494,7 @@
       <c r="J68" s="11"/>
       <c r="K68" s="20"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="40"/>
       <c r="B69" s="20"/>
       <c r="C69" s="13"/>
@@ -5498,7 +5510,7 @@
       <c r="J69" s="11"/>
       <c r="K69" s="20"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="40"/>
       <c r="B70" s="20"/>
       <c r="C70" s="13"/>
@@ -5514,7 +5526,7 @@
       <c r="J70" s="11"/>
       <c r="K70" s="20"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="40"/>
       <c r="B71" s="20"/>
       <c r="C71" s="13"/>
@@ -5530,7 +5542,7 @@
       <c r="J71" s="11"/>
       <c r="K71" s="20"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="40"/>
       <c r="B72" s="20"/>
       <c r="C72" s="13"/>
@@ -5546,7 +5558,7 @@
       <c r="J72" s="11"/>
       <c r="K72" s="20"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="40"/>
       <c r="B73" s="20"/>
       <c r="C73" s="13"/>
@@ -5562,7 +5574,7 @@
       <c r="J73" s="11"/>
       <c r="K73" s="20"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="40"/>
       <c r="B74" s="20"/>
       <c r="C74" s="13"/>
@@ -5578,7 +5590,7 @@
       <c r="J74" s="11"/>
       <c r="K74" s="20"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="41"/>
       <c r="B75" s="15"/>
       <c r="C75" s="42"/>
@@ -5609,10 +5621,10 @@
     <mergeCell ref="F4:G4"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"1 - Married (and not separated), 2 - Widowed (including living common law), 3 - Separated (including living common law), 4 - Divorced (including living common law), 5 - Single (including living common law)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:C4" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"PERMANENT, CO-TERMINUS, CASUAL, JOBCON"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5635,28 +5647,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="37" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" style="37" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D1" s="58" t="s">
         <v>33</v>
       </c>
@@ -5669,7 +5681,7 @@
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>24</v>
       </c>
@@ -5698,7 +5710,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>127.869</v>
       </c>
@@ -5726,17 +5738,20 @@
         <v>---</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="G4" s="33"/>
       <c r="J4" s="1" t="str">
         <f>IF(TEXT(J3,"D")=1,1,TEXT(J3,"D"))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>96</v>
+      </c>
       <c r="C6" s="38" t="s">
         <v>28</v>
       </c>
@@ -5757,7 +5772,11 @@
       <c r="K6" s="60"/>
       <c r="L6" s="60"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <f>SUM('2018 LEAVE CREDITS'!E9,'2018 LEAVE CREDITS'!I9)</f>
+        <v>129.89699999999999</v>
+      </c>
       <c r="C7" s="37">
         <v>1</v>
       </c>
@@ -5784,7 +5803,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8" s="37">
         <v>2</v>
       </c>
@@ -5810,7 +5829,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9" s="37">
         <v>3</v>
       </c>
@@ -5836,7 +5855,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10" s="37">
         <v>4</v>
       </c>
@@ -5862,7 +5881,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11" s="37">
         <v>5</v>
       </c>
@@ -5888,7 +5907,7 @@
         <v>0.16700000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12" s="37">
         <v>6</v>
       </c>
@@ -5914,7 +5933,7 @@
         <v>0.20800000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13" s="37">
         <v>7</v>
       </c>
@@ -5940,7 +5959,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="37">
         <v>8</v>
       </c>
@@ -5966,7 +5985,7 @@
         <v>0.29199999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15" s="37">
         <v>9</v>
       </c>
@@ -5986,7 +6005,7 @@
         <v>0.33299999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C16" s="37">
         <v>10</v>
       </c>
@@ -6006,7 +6025,7 @@
         <v>0.37499999999999994</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" s="37">
         <v>11</v>
       </c>
@@ -6026,7 +6045,7 @@
         <v>0.41699999999999993</v>
       </c>
     </row>
-    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C18" s="37">
         <v>12</v>
       </c>
@@ -6047,7 +6066,7 @@
         <v>0.45799999999999991</v>
       </c>
     </row>
-    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C19" s="37">
         <v>13</v>
       </c>
@@ -6068,7 +6087,7 @@
         <v>0.49999999999999989</v>
       </c>
     </row>
-    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C20" s="37">
         <v>14</v>
       </c>
@@ -6089,7 +6108,7 @@
         <v>0.54199999999999993</v>
       </c>
     </row>
-    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C21" s="37">
         <v>15</v>
       </c>
@@ -6110,7 +6129,7 @@
         <v>0.58299999999999996</v>
       </c>
     </row>
-    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C22" s="37">
         <v>16</v>
       </c>
@@ -6131,7 +6150,7 @@
         <v>0.625</v>
       </c>
     </row>
-    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="37">
         <v>17</v>
       </c>
@@ -6152,7 +6171,7 @@
         <v>0.66700000000000004</v>
       </c>
     </row>
-    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C24" s="37">
         <v>18</v>
       </c>
@@ -6173,7 +6192,7 @@
         <v>0.70800000000000007</v>
       </c>
     </row>
-    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C25" s="37">
         <v>19</v>
       </c>
@@ -6194,7 +6213,7 @@
         <v>0.75000000000000011</v>
       </c>
     </row>
-    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C26" s="37">
         <v>20</v>
       </c>
@@ -6215,7 +6234,7 @@
         <v>0.79200000000000015</v>
       </c>
     </row>
-    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C27" s="37">
         <v>21</v>
       </c>
@@ -6236,7 +6255,7 @@
         <v>0.83300000000000018</v>
       </c>
     </row>
-    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="37">
         <v>22</v>
       </c>
@@ -6257,7 +6276,7 @@
         <v>0.87500000000000022</v>
       </c>
     </row>
-    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C29" s="37">
         <v>23</v>
       </c>
@@ -6278,7 +6297,7 @@
         <v>0.91700000000000026</v>
       </c>
     </row>
-    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="37">
         <v>24</v>
       </c>
@@ -6299,7 +6318,7 @@
         <v>0.9580000000000003</v>
       </c>
     </row>
-    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C31" s="37">
         <v>25</v>
       </c>
@@ -6320,7 +6339,7 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C32" s="37">
         <v>26</v>
       </c>
@@ -6341,7 +6360,7 @@
         <v>1.0420000000000003</v>
       </c>
     </row>
-    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C33" s="37">
         <v>27</v>
       </c>
@@ -6362,7 +6381,7 @@
         <v>1.0830000000000002</v>
       </c>
     </row>
-    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C34" s="37">
         <v>28</v>
       </c>
@@ -6383,7 +6402,7 @@
         <v>1.1250000000000002</v>
       </c>
     </row>
-    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C35" s="37">
         <v>29</v>
       </c>
@@ -6404,7 +6423,7 @@
         <v>1.1670000000000003</v>
       </c>
     </row>
-    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C36" s="37">
         <v>30</v>
       </c>
@@ -6425,7 +6444,7 @@
         <v>1.2080000000000002</v>
       </c>
     </row>
-    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C37" s="37">
         <v>31</v>
       </c>
@@ -6446,7 +6465,7 @@
         <v>1.2500000000000002</v>
       </c>
     </row>
-    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C38" s="37">
         <v>32</v>
       </c>
@@ -6455,7 +6474,7 @@
       </c>
       <c r="G38"/>
     </row>
-    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C39" s="37">
         <v>33</v>
       </c>
@@ -6464,7 +6483,7 @@
       </c>
       <c r="G39"/>
     </row>
-    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C40" s="37">
         <v>34</v>
       </c>
@@ -6473,7 +6492,7 @@
       </c>
       <c r="G40"/>
     </row>
-    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C41" s="37">
         <v>35</v>
       </c>
@@ -6482,7 +6501,7 @@
       </c>
       <c r="G41"/>
     </row>
-    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C42" s="37">
         <v>36</v>
       </c>
@@ -6491,7 +6510,7 @@
       </c>
       <c r="G42"/>
     </row>
-    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C43" s="37">
         <v>37</v>
       </c>
@@ -6500,7 +6519,7 @@
       </c>
       <c r="G43"/>
     </row>
-    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C44" s="37">
         <v>38</v>
       </c>
@@ -6509,7 +6528,7 @@
       </c>
       <c r="G44"/>
     </row>
-    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C45" s="37">
         <v>39</v>
       </c>
@@ -6518,7 +6537,7 @@
       </c>
       <c r="G45"/>
     </row>
-    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C46" s="37">
         <v>40</v>
       </c>
@@ -6527,7 +6546,7 @@
       </c>
       <c r="G46"/>
     </row>
-    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C47" s="37">
         <v>41</v>
       </c>
@@ -6536,7 +6555,7 @@
       </c>
       <c r="G47"/>
     </row>
-    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C48" s="37">
         <v>42</v>
       </c>
@@ -6545,7 +6564,7 @@
       </c>
       <c r="G48"/>
     </row>
-    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C49" s="37">
         <v>43</v>
       </c>
@@ -6554,7 +6573,7 @@
       </c>
       <c r="G49"/>
     </row>
-    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C50" s="37">
         <v>44</v>
       </c>
@@ -6563,7 +6582,7 @@
       </c>
       <c r="G50"/>
     </row>
-    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C51" s="37">
         <v>45</v>
       </c>
@@ -6572,7 +6591,7 @@
       </c>
       <c r="G51"/>
     </row>
-    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C52" s="37">
         <v>46</v>
       </c>
@@ -6581,7 +6600,7 @@
       </c>
       <c r="G52"/>
     </row>
-    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C53" s="37">
         <v>47</v>
       </c>
@@ -6590,7 +6609,7 @@
       </c>
       <c r="G53"/>
     </row>
-    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C54" s="37">
         <v>48</v>
       </c>
@@ -6599,7 +6618,7 @@
       </c>
       <c r="G54"/>
     </row>
-    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C55" s="37">
         <v>49</v>
       </c>
@@ -6608,7 +6627,7 @@
       </c>
       <c r="G55"/>
     </row>
-    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C56" s="37">
         <v>50</v>
       </c>
@@ -6617,7 +6636,7 @@
       </c>
       <c r="G56"/>
     </row>
-    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C57" s="37">
         <v>51</v>
       </c>
@@ -6626,7 +6645,7 @@
       </c>
       <c r="G57"/>
     </row>
-    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="37">
         <v>52</v>
       </c>
@@ -6635,7 +6654,7 @@
       </c>
       <c r="G58"/>
     </row>
-    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C59" s="37">
         <v>53</v>
       </c>
@@ -6644,7 +6663,7 @@
       </c>
       <c r="G59"/>
     </row>
-    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C60" s="37">
         <v>54</v>
       </c>
@@ -6653,7 +6672,7 @@
       </c>
       <c r="G60"/>
     </row>
-    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C61" s="37">
         <v>55</v>
       </c>
@@ -6662,7 +6681,7 @@
       </c>
       <c r="G61"/>
     </row>
-    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C62" s="37">
         <v>56</v>
       </c>
@@ -6671,7 +6690,7 @@
       </c>
       <c r="G62"/>
     </row>
-    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C63" s="37">
         <v>57</v>
       </c>
@@ -6680,7 +6699,7 @@
       </c>
       <c r="G63"/>
     </row>
-    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C64" s="37">
         <v>58</v>
       </c>
@@ -6689,7 +6708,7 @@
       </c>
       <c r="G64"/>
     </row>
-    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C65" s="37">
         <v>59</v>
       </c>
@@ -6698,7 +6717,7 @@
       </c>
       <c r="G65"/>
     </row>
-    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C66" s="37">
         <v>60</v>
       </c>
@@ -6707,7 +6726,7 @@
       </c>
       <c r="G66"/>
     </row>
-    <row r="67" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>

</xml_diff>